<commit_message>
added data bars to estimated / actual time
</commit_message>
<xml_diff>
--- a/PhD Progress.xlsx
+++ b/PhD Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheilaannschoepp/Documents/phd_productivity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A7C9A9B-D66E-274D-B4A3-0FB5E3E4396E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5154874F-1BB1-2647-973E-7E676A0DECA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{D506D56E-27E5-7B4E-8CF4-861457431C2C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{D506D56E-27E5-7B4E-8CF4-861457431C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly PhD Tasks" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>Identifier</t>
   </si>
@@ -198,7 +198,22 @@
     <t>Value / Benefit of Achieving Task</t>
   </si>
   <si>
-    <t>Time (h:mm)</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Time (h)</t>
+  </si>
+  <si>
+    <t>CSGSA</t>
+  </si>
+  <si>
+    <t>Tasks related to the Computing Science Graduate Students' Association.</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Totals for applicable columns.</t>
   </si>
 </sst>
 </file>
@@ -247,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -435,11 +456,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="6" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -519,23 +555,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -594,78 +618,47 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color theme="0"/>
@@ -844,58 +837,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -915,87 +857,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1016,27 +878,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1047,249 +889,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1576,11 +1175,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8CD933-4FEF-AA44-936A-D3BD6CBCDACF}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1588,11 +1187,13 @@
     <col min="1" max="1" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="59" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="2" customWidth="1"/>
     <col min="8" max="10" width="42.83203125" style="2" customWidth="1"/>
-    <col min="11" max="12" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -1606,10 +1207,10 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -1627,8 +1228,8 @@
       <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
+      <c r="K1" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>9</v>
@@ -1644,11 +1245,11 @@
       <c r="C2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>53</v>
+      <c r="D2" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>54</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>29</v>
@@ -1663,40 +1264,42 @@
         <v>52</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="K2" s="50" t="s">
+        <v>30</v>
+      </c>
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="41"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="37"/>
     </row>
     <row r="4" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
@@ -1704,14 +1307,14 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="10"/>
       <c r="G5" s="13"/>
       <c r="H5" s="18"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="K5" s="52"/>
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1720,14 +1323,14 @@
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="11"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="11"/>
       <c r="G6" s="14"/>
       <c r="H6" s="19"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1736,14 +1339,14 @@
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="11"/>
       <c r="G7" s="14"/>
       <c r="H7" s="19"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1752,14 +1355,14 @@
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="11"/>
       <c r="G8" s="14"/>
       <c r="H8" s="19"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="14"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1768,14 +1371,14 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
       <c r="F9" s="11"/>
       <c r="G9" s="14"/>
       <c r="H9" s="19"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="14"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1784,14 +1387,14 @@
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="11"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="11"/>
       <c r="G10" s="14"/>
       <c r="H10" s="19"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1800,14 +1403,14 @@
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="11"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="11"/>
       <c r="G11" s="14"/>
       <c r="H11" s="19"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1816,14 +1419,14 @@
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="11"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
       <c r="F12" s="11"/>
       <c r="G12" s="14"/>
       <c r="H12" s="19"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="14"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1832,14 +1435,14 @@
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="11"/>
       <c r="G13" s="14"/>
       <c r="H13" s="19"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -1848,47 +1451,47 @@
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="12"/>
       <c r="G14" s="15"/>
       <c r="H14" s="20"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+      <c r="K14" s="17"/>
       <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31"/>
     </row>
     <row r="16" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="34"/>
     </row>
     <row r="17" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
@@ -1896,14 +1499,14 @@
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="10"/>
       <c r="G17" s="13"/>
       <c r="H17" s="18"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1912,14 +1515,14 @@
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="11"/>
       <c r="G18" s="14"/>
       <c r="H18" s="19"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1928,14 +1531,14 @@
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
       <c r="F19" s="11"/>
       <c r="G19" s="14"/>
       <c r="H19" s="19"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1944,14 +1547,14 @@
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
       <c r="F20" s="11"/>
       <c r="G20" s="14"/>
       <c r="H20" s="19"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
+      <c r="K20" s="16"/>
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1960,14 +1563,14 @@
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
       <c r="F21" s="11"/>
       <c r="G21" s="14"/>
       <c r="H21" s="19"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1976,14 +1579,14 @@
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
       <c r="F22" s="11"/>
       <c r="G22" s="14"/>
       <c r="H22" s="19"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1992,14 +1595,14 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
       <c r="F23" s="11"/>
       <c r="G23" s="14"/>
       <c r="H23" s="19"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2008,14 +1611,14 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="11"/>
       <c r="G24" s="14"/>
       <c r="H24" s="19"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
+      <c r="K24" s="16"/>
       <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2024,14 +1627,14 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
       <c r="F25" s="11"/>
       <c r="G25" s="14"/>
       <c r="H25" s="19"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2040,47 +1643,47 @@
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="12"/>
       <c r="G26" s="15"/>
       <c r="H26" s="20"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
+      <c r="K26" s="17"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="35"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="31"/>
     </row>
     <row r="28" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="38"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="34"/>
     </row>
     <row r="29" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
@@ -2088,14 +1691,14 @@
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
       <c r="F29" s="10"/>
       <c r="G29" s="13"/>
       <c r="H29" s="18"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="52"/>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2104,14 +1707,14 @@
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
       <c r="F30" s="11"/>
       <c r="G30" s="14"/>
       <c r="H30" s="19"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
+      <c r="K30" s="16"/>
       <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -2120,14 +1723,14 @@
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
       <c r="F31" s="11"/>
       <c r="G31" s="14"/>
       <c r="H31" s="19"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
+      <c r="K31" s="16"/>
       <c r="L31" s="14"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -2136,14 +1739,14 @@
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="11"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="11"/>
       <c r="G32" s="14"/>
       <c r="H32" s="19"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="14"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -2152,14 +1755,14 @@
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="11"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
       <c r="F33" s="11"/>
       <c r="G33" s="14"/>
       <c r="H33" s="19"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
+      <c r="K33" s="16"/>
       <c r="L33" s="14"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2168,14 +1771,14 @@
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
       <c r="F34" s="11"/>
       <c r="G34" s="14"/>
       <c r="H34" s="19"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
+      <c r="K34" s="16"/>
       <c r="L34" s="14"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -2184,14 +1787,14 @@
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
       <c r="F35" s="11"/>
       <c r="G35" s="14"/>
       <c r="H35" s="19"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
+      <c r="K35" s="16"/>
       <c r="L35" s="14"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -2200,14 +1803,14 @@
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="11"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
       <c r="F36" s="11"/>
       <c r="G36" s="14"/>
       <c r="H36" s="19"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
+      <c r="K36" s="16"/>
       <c r="L36" s="14"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2216,14 +1819,14 @@
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="11"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
       <c r="F37" s="11"/>
       <c r="G37" s="14"/>
       <c r="H37" s="19"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
+      <c r="K37" s="16"/>
       <c r="L37" s="14"/>
     </row>
     <row r="38" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2232,47 +1835,47 @@
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="12"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
       <c r="F38" s="12"/>
       <c r="G38" s="15"/>
       <c r="H38" s="20"/>
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="K38" s="17"/>
       <c r="L38" s="15"/>
     </row>
     <row r="39" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="35"/>
+      <c r="A39" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="31"/>
     </row>
     <row r="40" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="38"/>
+      <c r="A40" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="34"/>
     </row>
     <row r="41" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
@@ -2280,14 +1883,14 @@
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="10"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
       <c r="F41" s="10"/>
       <c r="G41" s="13"/>
       <c r="H41" s="18"/>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+      <c r="K41" s="52"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2296,14 +1899,14 @@
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="11"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
       <c r="F42" s="11"/>
       <c r="G42" s="14"/>
       <c r="H42" s="19"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
+      <c r="K42" s="16"/>
       <c r="L42" s="14"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2312,14 +1915,14 @@
       </c>
       <c r="B43" s="14"/>
       <c r="C43" s="11"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
       <c r="F43" s="11"/>
       <c r="G43" s="14"/>
       <c r="H43" s="19"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
+      <c r="K43" s="16"/>
       <c r="L43" s="14"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2328,14 +1931,14 @@
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="11"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
       <c r="F44" s="11"/>
       <c r="G44" s="14"/>
       <c r="H44" s="19"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="K44" s="16"/>
       <c r="L44" s="14"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2344,14 +1947,14 @@
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="11"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
       <c r="F45" s="11"/>
       <c r="G45" s="14"/>
       <c r="H45" s="19"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
+      <c r="K45" s="16"/>
       <c r="L45" s="14"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2360,14 +1963,14 @@
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="11"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
       <c r="F46" s="11"/>
       <c r="G46" s="14"/>
       <c r="H46" s="19"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
+      <c r="K46" s="16"/>
       <c r="L46" s="14"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2376,14 +1979,14 @@
       </c>
       <c r="B47" s="14"/>
       <c r="C47" s="11"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
       <c r="F47" s="11"/>
       <c r="G47" s="14"/>
       <c r="H47" s="19"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
+      <c r="K47" s="16"/>
       <c r="L47" s="14"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2392,14 +1995,14 @@
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="11"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
       <c r="F48" s="11"/>
       <c r="G48" s="14"/>
       <c r="H48" s="19"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
+      <c r="K48" s="16"/>
       <c r="L48" s="14"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -2408,14 +2011,14 @@
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="11"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
       <c r="F49" s="11"/>
       <c r="G49" s="14"/>
       <c r="H49" s="19"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
+      <c r="K49" s="16"/>
       <c r="L49" s="14"/>
     </row>
     <row r="50" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2424,47 +2027,47 @@
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="12"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
       <c r="F50" s="12"/>
       <c r="G50" s="15"/>
       <c r="H50" s="20"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
+      <c r="K50" s="17"/>
       <c r="L50" s="15"/>
     </row>
     <row r="51" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="35"/>
+      <c r="A51" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="31"/>
     </row>
     <row r="52" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="38"/>
+      <c r="A52" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="34"/>
     </row>
     <row r="53" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10">
@@ -2472,14 +2075,14 @@
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="10"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
       <c r="F53" s="10"/>
       <c r="G53" s="13"/>
       <c r="H53" s="18"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
+      <c r="K53" s="52"/>
       <c r="L53" s="13"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -2488,14 +2091,14 @@
       </c>
       <c r="B54" s="14"/>
       <c r="C54" s="11"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
       <c r="F54" s="11"/>
       <c r="G54" s="14"/>
       <c r="H54" s="19"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
+      <c r="K54" s="16"/>
       <c r="L54" s="14"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -2504,14 +2107,14 @@
       </c>
       <c r="B55" s="14"/>
       <c r="C55" s="11"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
       <c r="F55" s="11"/>
       <c r="G55" s="14"/>
       <c r="H55" s="19"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
+      <c r="K55" s="16"/>
       <c r="L55" s="14"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -2520,14 +2123,14 @@
       </c>
       <c r="B56" s="14"/>
       <c r="C56" s="11"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
       <c r="F56" s="11"/>
       <c r="G56" s="14"/>
       <c r="H56" s="19"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
+      <c r="K56" s="16"/>
       <c r="L56" s="14"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -2536,14 +2139,14 @@
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="11"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
       <c r="F57" s="11"/>
       <c r="G57" s="14"/>
       <c r="H57" s="19"/>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
+      <c r="K57" s="16"/>
       <c r="L57" s="14"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
@@ -2552,14 +2155,14 @@
       </c>
       <c r="B58" s="14"/>
       <c r="C58" s="11"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
       <c r="F58" s="11"/>
       <c r="G58" s="14"/>
       <c r="H58" s="19"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
+      <c r="K58" s="16"/>
       <c r="L58" s="14"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -2568,14 +2171,14 @@
       </c>
       <c r="B59" s="14"/>
       <c r="C59" s="11"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
       <c r="F59" s="11"/>
       <c r="G59" s="14"/>
       <c r="H59" s="19"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
+      <c r="K59" s="16"/>
       <c r="L59" s="14"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -2584,14 +2187,14 @@
       </c>
       <c r="B60" s="14"/>
       <c r="C60" s="11"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
       <c r="F60" s="11"/>
       <c r="G60" s="14"/>
       <c r="H60" s="19"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
+      <c r="K60" s="16"/>
       <c r="L60" s="14"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -2600,14 +2203,14 @@
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="11"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
       <c r="F61" s="11"/>
       <c r="G61" s="14"/>
       <c r="H61" s="19"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
+      <c r="K61" s="16"/>
       <c r="L61" s="14"/>
     </row>
     <row r="62" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2616,47 +2219,47 @@
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="12"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="54"/>
       <c r="F62" s="12"/>
       <c r="G62" s="15"/>
       <c r="H62" s="20"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
-      <c r="K62" s="15"/>
+      <c r="K62" s="17"/>
       <c r="L62" s="15"/>
     </row>
     <row r="63" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="35"/>
+      <c r="A63" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="30"/>
+      <c r="L63" s="31"/>
     </row>
     <row r="64" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="37"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="37"/>
-      <c r="L64" s="38"/>
+      <c r="A64" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="34"/>
     </row>
     <row r="65" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="10">
@@ -2664,14 +2267,14 @@
       </c>
       <c r="B65" s="13"/>
       <c r="C65" s="10"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
       <c r="F65" s="10"/>
       <c r="G65" s="13"/>
       <c r="H65" s="18"/>
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
+      <c r="K65" s="52"/>
       <c r="L65" s="13"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
@@ -2680,14 +2283,14 @@
       </c>
       <c r="B66" s="14"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="53"/>
       <c r="F66" s="11"/>
       <c r="G66" s="14"/>
       <c r="H66" s="19"/>
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
+      <c r="K66" s="16"/>
       <c r="L66" s="14"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -2696,14 +2299,14 @@
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
       <c r="F67" s="11"/>
       <c r="G67" s="14"/>
       <c r="H67" s="19"/>
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
+      <c r="K67" s="16"/>
       <c r="L67" s="14"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -2712,14 +2315,14 @@
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="11"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="53"/>
       <c r="F68" s="11"/>
       <c r="G68" s="14"/>
       <c r="H68" s="19"/>
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
+      <c r="K68" s="16"/>
       <c r="L68" s="14"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -2728,14 +2331,14 @@
       </c>
       <c r="B69" s="14"/>
       <c r="C69" s="11"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
       <c r="F69" s="11"/>
       <c r="G69" s="14"/>
       <c r="H69" s="19"/>
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
+      <c r="K69" s="16"/>
       <c r="L69" s="14"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -2744,14 +2347,14 @@
       </c>
       <c r="B70" s="14"/>
       <c r="C70" s="11"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
       <c r="F70" s="11"/>
       <c r="G70" s="14"/>
       <c r="H70" s="19"/>
       <c r="I70" s="14"/>
       <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
+      <c r="K70" s="16"/>
       <c r="L70" s="14"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -2760,14 +2363,14 @@
       </c>
       <c r="B71" s="14"/>
       <c r="C71" s="11"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
       <c r="F71" s="11"/>
       <c r="G71" s="14"/>
       <c r="H71" s="19"/>
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
+      <c r="K71" s="16"/>
       <c r="L71" s="14"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -2776,14 +2379,14 @@
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="11"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
+      <c r="D72" s="53"/>
+      <c r="E72" s="53"/>
       <c r="F72" s="11"/>
       <c r="G72" s="14"/>
       <c r="H72" s="19"/>
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
+      <c r="K72" s="16"/>
       <c r="L72" s="14"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
@@ -2792,14 +2395,14 @@
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="11"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="53"/>
       <c r="F73" s="11"/>
       <c r="G73" s="14"/>
       <c r="H73" s="19"/>
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
+      <c r="K73" s="16"/>
       <c r="L73" s="14"/>
     </row>
     <row r="74" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -2808,47 +2411,47 @@
       </c>
       <c r="B74" s="15"/>
       <c r="C74" s="12"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="31"/>
+      <c r="D74" s="54"/>
+      <c r="E74" s="54"/>
       <c r="F74" s="12"/>
       <c r="G74" s="15"/>
       <c r="H74" s="20"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
+      <c r="K74" s="17"/>
       <c r="L74" s="15"/>
     </row>
     <row r="75" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="34"/>
-      <c r="K75" s="34"/>
-      <c r="L75" s="35"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+      <c r="L75" s="31"/>
     </row>
     <row r="76" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="36" t="s">
+      <c r="A76" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="37"/>
-      <c r="I76" s="37"/>
-      <c r="J76" s="37"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="38"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="34"/>
     </row>
     <row r="77" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
@@ -2856,14 +2459,14 @@
       </c>
       <c r="B77" s="13"/>
       <c r="C77" s="10"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
+      <c r="D77" s="51"/>
+      <c r="E77" s="51"/>
       <c r="F77" s="10"/>
       <c r="G77" s="13"/>
       <c r="H77" s="18"/>
       <c r="I77" s="13"/>
       <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
+      <c r="K77" s="52"/>
       <c r="L77" s="13"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -2872,14 +2475,14 @@
       </c>
       <c r="B78" s="14"/>
       <c r="C78" s="11"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
+      <c r="D78" s="53"/>
+      <c r="E78" s="53"/>
       <c r="F78" s="11"/>
       <c r="G78" s="14"/>
       <c r="H78" s="19"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
-      <c r="K78" s="14"/>
+      <c r="K78" s="16"/>
       <c r="L78" s="14"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -2888,14 +2491,14 @@
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="11"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
+      <c r="D79" s="53"/>
+      <c r="E79" s="53"/>
       <c r="F79" s="11"/>
       <c r="G79" s="14"/>
       <c r="H79" s="19"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
+      <c r="K79" s="16"/>
       <c r="L79" s="14"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -2904,14 +2507,14 @@
       </c>
       <c r="B80" s="14"/>
       <c r="C80" s="11"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="53"/>
       <c r="F80" s="11"/>
       <c r="G80" s="14"/>
       <c r="H80" s="19"/>
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
-      <c r="K80" s="14"/>
+      <c r="K80" s="16"/>
       <c r="L80" s="14"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
@@ -2920,14 +2523,14 @@
       </c>
       <c r="B81" s="14"/>
       <c r="C81" s="11"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
+      <c r="D81" s="53"/>
+      <c r="E81" s="53"/>
       <c r="F81" s="11"/>
       <c r="G81" s="14"/>
       <c r="H81" s="19"/>
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
+      <c r="K81" s="16"/>
       <c r="L81" s="14"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
@@ -2936,14 +2539,14 @@
       </c>
       <c r="B82" s="14"/>
       <c r="C82" s="11"/>
-      <c r="D82" s="30"/>
-      <c r="E82" s="30"/>
+      <c r="D82" s="53"/>
+      <c r="E82" s="53"/>
       <c r="F82" s="11"/>
       <c r="G82" s="14"/>
       <c r="H82" s="19"/>
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
-      <c r="K82" s="14"/>
+      <c r="K82" s="16"/>
       <c r="L82" s="14"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
@@ -2952,14 +2555,14 @@
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="11"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="30"/>
+      <c r="D83" s="53"/>
+      <c r="E83" s="53"/>
       <c r="F83" s="11"/>
       <c r="G83" s="14"/>
       <c r="H83" s="19"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
-      <c r="K83" s="14"/>
+      <c r="K83" s="16"/>
       <c r="L83" s="14"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -2968,14 +2571,14 @@
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="11"/>
-      <c r="D84" s="30"/>
-      <c r="E84" s="30"/>
+      <c r="D84" s="53"/>
+      <c r="E84" s="53"/>
       <c r="F84" s="11"/>
       <c r="G84" s="14"/>
       <c r="H84" s="19"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
+      <c r="K84" s="16"/>
       <c r="L84" s="14"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
@@ -2984,14 +2587,14 @@
       </c>
       <c r="B85" s="14"/>
       <c r="C85" s="11"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
       <c r="F85" s="11"/>
       <c r="G85" s="14"/>
       <c r="H85" s="19"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
-      <c r="K85" s="14"/>
+      <c r="K85" s="16"/>
       <c r="L85" s="14"/>
     </row>
     <row r="86" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -3000,19 +2603,267 @@
       </c>
       <c r="B86" s="15"/>
       <c r="C86" s="12"/>
-      <c r="D86" s="31"/>
-      <c r="E86" s="31"/>
+      <c r="D86" s="54"/>
+      <c r="E86" s="54"/>
       <c r="F86" s="12"/>
       <c r="G86" s="15"/>
       <c r="H86" s="20"/>
       <c r="I86" s="15"/>
       <c r="J86" s="15"/>
-      <c r="K86" s="15"/>
+      <c r="K86" s="17"/>
       <c r="L86" s="15"/>
     </row>
-    <row r="87" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30"/>
+      <c r="I87" s="30"/>
+      <c r="J87" s="30"/>
+      <c r="K87" s="30"/>
+      <c r="L87" s="31"/>
+    </row>
+    <row r="88" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="33"/>
+      <c r="K88" s="33"/>
+      <c r="L88" s="34"/>
+    </row>
+    <row r="89" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="10">
+        <v>1</v>
+      </c>
+      <c r="B89" s="13"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="51"/>
+      <c r="E89" s="51"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="52"/>
+      <c r="L89" s="13"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A90" s="11">
+        <v>2</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="53"/>
+      <c r="E90" s="53"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="14"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A91" s="11">
+        <v>3</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="53"/>
+      <c r="E91" s="53"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="14"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" s="11">
+        <v>4</v>
+      </c>
+      <c r="B92" s="14"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="53"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="14"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A93" s="11">
+        <v>5</v>
+      </c>
+      <c r="B93" s="14"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="53"/>
+      <c r="E93" s="53"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="16"/>
+      <c r="L93" s="14"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" s="11">
+        <v>6</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="53"/>
+      <c r="E94" s="53"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="19"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="16"/>
+      <c r="L94" s="14"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" s="11">
+        <v>7</v>
+      </c>
+      <c r="B95" s="14"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="53"/>
+      <c r="E95" s="53"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="19"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="16"/>
+      <c r="L95" s="14"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96" s="11">
+        <v>8</v>
+      </c>
+      <c r="B96" s="14"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="53"/>
+      <c r="E96" s="53"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="14"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" s="11">
+        <v>9</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="53"/>
+      <c r="E97" s="53"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="16"/>
+      <c r="L97" s="14"/>
+    </row>
+    <row r="98" spans="1:12" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="11">
+        <v>10</v>
+      </c>
+      <c r="B98" s="14"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="53"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="20"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="15"/>
+    </row>
+    <row r="99" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B99" s="30"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="30"/>
+      <c r="G99" s="30"/>
+      <c r="H99" s="30"/>
+      <c r="I99" s="30"/>
+      <c r="J99" s="30"/>
+      <c r="K99" s="30"/>
+      <c r="L99" s="31"/>
+    </row>
+    <row r="100" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
+      <c r="G100" s="33"/>
+      <c r="H100" s="33"/>
+      <c r="I100" s="33"/>
+      <c r="J100" s="33"/>
+      <c r="K100" s="33"/>
+      <c r="L100" s="34"/>
+    </row>
+    <row r="101" spans="1:12" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="55"/>
+      <c r="B101" s="56"/>
+      <c r="C101" s="55"/>
+      <c r="D101" s="57">
+        <f>SUM(D5:D14,D17:D26,D29:D38,D41:D50,D53:D62,D65:D74,D77:D86,D89:D98)</f>
+        <v>0</v>
+      </c>
+      <c r="E101" s="57">
+        <f>SUM(E5:E14,E17:E26,E29:E38,E41:E50,E53:E62,E65:E74,E77:E86,E89:E98)</f>
+        <v>0</v>
+      </c>
+      <c r="F101" s="55"/>
+      <c r="G101" s="56"/>
+      <c r="H101" s="56"/>
+      <c r="I101" s="56"/>
+      <c r="J101" s="56"/>
+      <c r="K101" s="58"/>
+      <c r="L101" s="56"/>
+    </row>
+    <row r="102" spans="1:12" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="18">
+    <mergeCell ref="A87:L87"/>
+    <mergeCell ref="A88:L88"/>
+    <mergeCell ref="A99:L99"/>
+    <mergeCell ref="A100:L100"/>
     <mergeCell ref="A75:L75"/>
     <mergeCell ref="A76:L76"/>
     <mergeCell ref="A64:L64"/>
@@ -3028,30 +2879,30 @@
     <mergeCell ref="A52:L52"/>
     <mergeCell ref="A63:L63"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:C14 C17:C26 C29:C38 C41:C50 C53:C62 C65:C74 C77:C86">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Low">
+  <conditionalFormatting sqref="C5:C14 C17:C26 C53:C62 C65:C74 C29:C50 C77:C86 C89:C98">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F14 F17:F26 F29:F38 F41:F50 F53:F62 F65:F74 F77:F86">
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Completed">
+  <conditionalFormatting sqref="F5:F14 F17:F26 F53:F62 F65:F74 F29:F50 F77:F86 F89:F98">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G14 G17:G26 G29:G38 G41:G50 G53:G62 G65:G74 G77:G86">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="G5:G14 G17:G26 G53:G62 G65:G74 G29:G50 G77:G86 G89:G98">
+    <cfRule type="dataBar" priority="3">
       <dataBar showValue="0">
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3059,19 +2910,47 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D2C73E6E-F096-1C42-B127-868ED10DF3BA}</x14:id>
+          <x14:id>{A7810DC7-3760-A049-8EF8-6458B27A3A01}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D14 D17:D26 D29:D38 D41:D50 D53:D62 D65:D74 D77:D86 D89:D98">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="formula" val="$D$101"/>
+        <color theme="8" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{46421054-2D76-1A4E-9FCC-F87EFE36C690}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E14 E17:E26 E29:E38 E41:E50 E53:E62 E65:E74 E77:E86 E89:E98">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="formula" val="$E$101"/>
+        <color theme="8" tint="0.39997558519241921"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{01BE39F6-F821-B44F-B78F-BB379E403F39}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14 C65:C74 C17:C26 C29:C38 C41:C50 C53:C62 C77:C86" xr:uid="{5573D0E8-1A89-B84E-8EB1-868966F8F87F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14 C17:C26 C29:C50 C53:C62 C65:C74 C77:C86 C89:C98" xr:uid="{61C9F866-30E2-3245-82C3-30C84CBE2528}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F14 F65:F74 F17:F26 F29:F38 F41:F50 F53:F62 F77:F86" xr:uid="{EC646072-4E84-A64E-A723-3399EE06C664}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F14 F17:F26 F29:F50 F53:F62 F65:F74 F77:F86 F89:F98" xr:uid="{8178AF88-2357-464A-ADE5-1BB2649F91AC}">
       <formula1>"Not Started,In Progress,Completed,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:C28 F27:F28" xr:uid="{83754121-FE98-2347-8240-FE0AF414C5A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27:C28 F27:F28" xr:uid="{E04A147E-A907-5F4E-AC24-E63F94BE1F2B}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -3081,7 +2960,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D2C73E6E-F096-1C42-B127-868ED10DF3BA}">
+          <x14:cfRule type="dataBar" id="{A7810DC7-3760-A049-8EF8-6458B27A3A01}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0" direction="leftToRight">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3093,7 +2972,37 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G5:G14 G17:G26 G29:G38 G41:G50 G53:G62 G65:G74 G77:G86</xm:sqref>
+          <xm:sqref>G5:G14 G17:G26 G53:G62 G65:G74 G29:G50 G77:G86 G89:G98</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{46421054-2D76-1A4E-9FCC-F87EFE36C690}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>$D$101</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor theme="5" tint="0.39997558519241921"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D5:D14 D17:D26 D29:D38 D41:D50 D53:D62 D65:D74 D77:D86 D89:D98</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{01BE39F6-F821-B44F-B78F-BB379E403F39}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>$E$101</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor theme="5" tint="0.39997558519241921"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E5:E14 E17:E26 E29:E38 E41:E50 E53:E62 E65:E74 E77:E86 E89:E98</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3106,7 +3015,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
@@ -3121,7 +3030,7 @@
     <col min="7" max="7" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="44.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="40.83203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="53" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="28" customWidth="1"/>
     <col min="12" max="12" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.1640625" style="4" customWidth="1"/>
     <col min="14" max="14" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -3162,14 +3071,14 @@
       <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="44"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="40"/>
       <c r="Q1" s="5" t="s">
         <v>9</v>
       </c>
@@ -3206,7 +3115,7 @@
         <v>31</v>
       </c>
       <c r="J2" s="23"/>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="27" t="s">
         <v>30</v>
       </c>
       <c r="L2" s="8" t="s">
@@ -3228,48 +3137,48 @@
       <c r="R2" s="23"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="50"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="46"/>
     </row>
     <row r="4" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="47"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
@@ -3491,48 +3400,48 @@
       <c r="R14" s="14"/>
     </row>
     <row r="15" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="35"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="31"/>
     </row>
     <row r="16" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="38"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="34"/>
     </row>
     <row r="17" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
@@ -3755,48 +3664,48 @@
       <c r="R26" s="14"/>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="35"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="31"/>
     </row>
     <row r="28" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="38"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="34"/>
     </row>
     <row r="29" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
@@ -4019,48 +3928,48 @@
       <c r="R38" s="14"/>
     </row>
     <row r="39" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="35"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="31"/>
     </row>
     <row r="40" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="46"/>
-      <c r="P40" s="46"/>
-      <c r="Q40" s="46"/>
-      <c r="R40" s="47"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="43"/>
     </row>
     <row r="41" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
@@ -4283,48 +4192,48 @@
       <c r="R50" s="14"/>
     </row>
     <row r="51" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
+      <c r="A51" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="34"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="34"/>
-      <c r="P51" s="34"/>
-      <c r="Q51" s="34"/>
-      <c r="R51" s="35"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="30"/>
+      <c r="M51" s="30"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="R51" s="31"/>
     </row>
     <row r="52" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
-      <c r="M52" s="37"/>
-      <c r="N52" s="37"/>
-      <c r="O52" s="37"/>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="37"/>
-      <c r="R52" s="38"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="33"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+      <c r="Q52" s="33"/>
+      <c r="R52" s="34"/>
     </row>
     <row r="53" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
@@ -4547,48 +4456,48 @@
       <c r="R62" s="14"/>
     </row>
     <row r="63" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="34"/>
-      <c r="O63" s="34"/>
-      <c r="P63" s="34"/>
-      <c r="Q63" s="34"/>
-      <c r="R63" s="35"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="30"/>
+      <c r="L63" s="30"/>
+      <c r="M63" s="30"/>
+      <c r="N63" s="30"/>
+      <c r="O63" s="30"/>
+      <c r="P63" s="30"/>
+      <c r="Q63" s="30"/>
+      <c r="R63" s="31"/>
     </row>
     <row r="64" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="36" t="s">
+      <c r="A64" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="37"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="37"/>
-      <c r="L64" s="37"/>
-      <c r="M64" s="37"/>
-      <c r="N64" s="37"/>
-      <c r="O64" s="37"/>
-      <c r="P64" s="37"/>
-      <c r="Q64" s="37"/>
-      <c r="R64" s="38"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="33"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="33"/>
+      <c r="Q64" s="33"/>
+      <c r="R64" s="34"/>
     </row>
     <row r="65" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
@@ -4811,48 +4720,48 @@
       <c r="R74" s="14"/>
     </row>
     <row r="75" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="34"/>
-      <c r="K75" s="34"/>
-      <c r="L75" s="34"/>
-      <c r="M75" s="34"/>
-      <c r="N75" s="34"/>
-      <c r="O75" s="34"/>
-      <c r="P75" s="34"/>
-      <c r="Q75" s="34"/>
-      <c r="R75" s="35"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="30"/>
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+      <c r="L75" s="30"/>
+      <c r="M75" s="30"/>
+      <c r="N75" s="30"/>
+      <c r="O75" s="30"/>
+      <c r="P75" s="30"/>
+      <c r="Q75" s="30"/>
+      <c r="R75" s="31"/>
     </row>
     <row r="76" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="36" t="s">
+      <c r="A76" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="37"/>
-      <c r="I76" s="37"/>
-      <c r="J76" s="37"/>
-      <c r="K76" s="37"/>
-      <c r="L76" s="37"/>
-      <c r="M76" s="37"/>
-      <c r="N76" s="37"/>
-      <c r="O76" s="37"/>
-      <c r="P76" s="37"/>
-      <c r="Q76" s="37"/>
-      <c r="R76" s="38"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="33"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="33"/>
+      <c r="O76" s="33"/>
+      <c r="P76" s="33"/>
+      <c r="Q76" s="33"/>
+      <c r="R76" s="34"/>
     </row>
     <row r="77" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
@@ -5075,48 +4984,48 @@
       <c r="R86" s="14"/>
     </row>
     <row r="87" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="33" t="s">
+      <c r="A87" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="34"/>
-      <c r="C87" s="34"/>
-      <c r="D87" s="34"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="34"/>
-      <c r="H87" s="34"/>
-      <c r="I87" s="34"/>
-      <c r="J87" s="34"/>
-      <c r="K87" s="34"/>
-      <c r="L87" s="34"/>
-      <c r="M87" s="34"/>
-      <c r="N87" s="34"/>
-      <c r="O87" s="34"/>
-      <c r="P87" s="34"/>
-      <c r="Q87" s="34"/>
-      <c r="R87" s="35"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30"/>
+      <c r="I87" s="30"/>
+      <c r="J87" s="30"/>
+      <c r="K87" s="30"/>
+      <c r="L87" s="30"/>
+      <c r="M87" s="30"/>
+      <c r="N87" s="30"/>
+      <c r="O87" s="30"/>
+      <c r="P87" s="30"/>
+      <c r="Q87" s="30"/>
+      <c r="R87" s="31"/>
     </row>
     <row r="88" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="36" t="s">
+      <c r="A88" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
-      <c r="G88" s="37"/>
-      <c r="H88" s="37"/>
-      <c r="I88" s="37"/>
-      <c r="J88" s="37"/>
-      <c r="K88" s="37"/>
-      <c r="L88" s="37"/>
-      <c r="M88" s="37"/>
-      <c r="N88" s="37"/>
-      <c r="O88" s="37"/>
-      <c r="P88" s="37"/>
-      <c r="Q88" s="37"/>
-      <c r="R88" s="38"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="33"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="33"/>
+      <c r="K88" s="33"/>
+      <c r="L88" s="33"/>
+      <c r="M88" s="33"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="33"/>
+      <c r="P88" s="33"/>
+      <c r="Q88" s="33"/>
+      <c r="R88" s="34"/>
     </row>
     <row r="89" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
@@ -5339,48 +5248,48 @@
       <c r="R98" s="14"/>
     </row>
     <row r="99" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="33" t="s">
+      <c r="A99" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B99" s="34"/>
-      <c r="C99" s="34"/>
-      <c r="D99" s="34"/>
-      <c r="E99" s="34"/>
-      <c r="F99" s="34"/>
-      <c r="G99" s="34"/>
-      <c r="H99" s="34"/>
-      <c r="I99" s="34"/>
-      <c r="J99" s="34"/>
-      <c r="K99" s="34"/>
-      <c r="L99" s="34"/>
-      <c r="M99" s="34"/>
-      <c r="N99" s="34"/>
-      <c r="O99" s="34"/>
-      <c r="P99" s="34"/>
-      <c r="Q99" s="34"/>
-      <c r="R99" s="35"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="30"/>
+      <c r="F99" s="30"/>
+      <c r="G99" s="30"/>
+      <c r="H99" s="30"/>
+      <c r="I99" s="30"/>
+      <c r="J99" s="30"/>
+      <c r="K99" s="30"/>
+      <c r="L99" s="30"/>
+      <c r="M99" s="30"/>
+      <c r="N99" s="30"/>
+      <c r="O99" s="30"/>
+      <c r="P99" s="30"/>
+      <c r="Q99" s="30"/>
+      <c r="R99" s="31"/>
     </row>
     <row r="100" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="36" t="s">
+      <c r="A100" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B100" s="37"/>
-      <c r="C100" s="37"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="37"/>
-      <c r="H100" s="37"/>
-      <c r="I100" s="37"/>
-      <c r="J100" s="37"/>
-      <c r="K100" s="37"/>
-      <c r="L100" s="37"/>
-      <c r="M100" s="37"/>
-      <c r="N100" s="37"/>
-      <c r="O100" s="37"/>
-      <c r="P100" s="37"/>
-      <c r="Q100" s="37"/>
-      <c r="R100" s="38"/>
+      <c r="B100" s="33"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
+      <c r="G100" s="33"/>
+      <c r="H100" s="33"/>
+      <c r="I100" s="33"/>
+      <c r="J100" s="33"/>
+      <c r="K100" s="33"/>
+      <c r="L100" s="33"/>
+      <c r="M100" s="33"/>
+      <c r="N100" s="33"/>
+      <c r="O100" s="33"/>
+      <c r="P100" s="33"/>
+      <c r="Q100" s="33"/>
+      <c r="R100" s="34"/>
     </row>
     <row r="101" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11">
@@ -5603,48 +5512,48 @@
       <c r="R110" s="14"/>
     </row>
     <row r="111" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="33" t="s">
+      <c r="A111" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B111" s="34"/>
-      <c r="C111" s="34"/>
-      <c r="D111" s="34"/>
-      <c r="E111" s="34"/>
-      <c r="F111" s="34"/>
-      <c r="G111" s="34"/>
-      <c r="H111" s="34"/>
-      <c r="I111" s="34"/>
-      <c r="J111" s="34"/>
-      <c r="K111" s="34"/>
-      <c r="L111" s="34"/>
-      <c r="M111" s="34"/>
-      <c r="N111" s="34"/>
-      <c r="O111" s="34"/>
-      <c r="P111" s="34"/>
-      <c r="Q111" s="34"/>
-      <c r="R111" s="35"/>
+      <c r="B111" s="30"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="30"/>
+      <c r="F111" s="30"/>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
+      <c r="I111" s="30"/>
+      <c r="J111" s="30"/>
+      <c r="K111" s="30"/>
+      <c r="L111" s="30"/>
+      <c r="M111" s="30"/>
+      <c r="N111" s="30"/>
+      <c r="O111" s="30"/>
+      <c r="P111" s="30"/>
+      <c r="Q111" s="30"/>
+      <c r="R111" s="31"/>
     </row>
     <row r="112" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="36" t="s">
+      <c r="A112" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B112" s="37"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="37"/>
-      <c r="E112" s="37"/>
-      <c r="F112" s="37"/>
-      <c r="G112" s="37"/>
-      <c r="H112" s="37"/>
-      <c r="I112" s="37"/>
-      <c r="J112" s="37"/>
-      <c r="K112" s="37"/>
-      <c r="L112" s="37"/>
-      <c r="M112" s="37"/>
-      <c r="N112" s="37"/>
-      <c r="O112" s="37"/>
-      <c r="P112" s="37"/>
-      <c r="Q112" s="37"/>
-      <c r="R112" s="38"/>
+      <c r="B112" s="33"/>
+      <c r="C112" s="33"/>
+      <c r="D112" s="33"/>
+      <c r="E112" s="33"/>
+      <c r="F112" s="33"/>
+      <c r="G112" s="33"/>
+      <c r="H112" s="33"/>
+      <c r="I112" s="33"/>
+      <c r="J112" s="33"/>
+      <c r="K112" s="33"/>
+      <c r="L112" s="33"/>
+      <c r="M112" s="33"/>
+      <c r="N112" s="33"/>
+      <c r="O112" s="33"/>
+      <c r="P112" s="33"/>
+      <c r="Q112" s="33"/>
+      <c r="R112" s="34"/>
     </row>
     <row r="113" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11">
@@ -5867,48 +5776,48 @@
       <c r="R122" s="14"/>
     </row>
     <row r="123" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="33" t="s">
+      <c r="A123" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B123" s="34"/>
-      <c r="C123" s="34"/>
-      <c r="D123" s="34"/>
-      <c r="E123" s="34"/>
-      <c r="F123" s="34"/>
-      <c r="G123" s="34"/>
-      <c r="H123" s="34"/>
-      <c r="I123" s="34"/>
-      <c r="J123" s="34"/>
-      <c r="K123" s="34"/>
-      <c r="L123" s="34"/>
-      <c r="M123" s="34"/>
-      <c r="N123" s="34"/>
-      <c r="O123" s="34"/>
-      <c r="P123" s="34"/>
-      <c r="Q123" s="34"/>
-      <c r="R123" s="35"/>
+      <c r="B123" s="30"/>
+      <c r="C123" s="30"/>
+      <c r="D123" s="30"/>
+      <c r="E123" s="30"/>
+      <c r="F123" s="30"/>
+      <c r="G123" s="30"/>
+      <c r="H123" s="30"/>
+      <c r="I123" s="30"/>
+      <c r="J123" s="30"/>
+      <c r="K123" s="30"/>
+      <c r="L123" s="30"/>
+      <c r="M123" s="30"/>
+      <c r="N123" s="30"/>
+      <c r="O123" s="30"/>
+      <c r="P123" s="30"/>
+      <c r="Q123" s="30"/>
+      <c r="R123" s="31"/>
     </row>
     <row r="124" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="36" t="s">
+      <c r="A124" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="37"/>
-      <c r="C124" s="37"/>
-      <c r="D124" s="37"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="37"/>
-      <c r="H124" s="37"/>
-      <c r="I124" s="37"/>
-      <c r="J124" s="37"/>
-      <c r="K124" s="37"/>
-      <c r="L124" s="37"/>
-      <c r="M124" s="37"/>
-      <c r="N124" s="37"/>
-      <c r="O124" s="37"/>
-      <c r="P124" s="37"/>
-      <c r="Q124" s="37"/>
-      <c r="R124" s="38"/>
+      <c r="B124" s="33"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
+      <c r="F124" s="33"/>
+      <c r="G124" s="33"/>
+      <c r="H124" s="33"/>
+      <c r="I124" s="33"/>
+      <c r="J124" s="33"/>
+      <c r="K124" s="33"/>
+      <c r="L124" s="33"/>
+      <c r="M124" s="33"/>
+      <c r="N124" s="33"/>
+      <c r="O124" s="33"/>
+      <c r="P124" s="33"/>
+      <c r="Q124" s="33"/>
+      <c r="R124" s="34"/>
     </row>
     <row r="125" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A125" s="11">
@@ -6131,48 +6040,48 @@
       <c r="R134" s="14"/>
     </row>
     <row r="135" spans="1:18" s="1" customFormat="1" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="33" t="s">
+      <c r="A135" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B135" s="34"/>
-      <c r="C135" s="34"/>
-      <c r="D135" s="34"/>
-      <c r="E135" s="34"/>
-      <c r="F135" s="34"/>
-      <c r="G135" s="34"/>
-      <c r="H135" s="34"/>
-      <c r="I135" s="34"/>
-      <c r="J135" s="34"/>
-      <c r="K135" s="34"/>
-      <c r="L135" s="34"/>
-      <c r="M135" s="34"/>
-      <c r="N135" s="34"/>
-      <c r="O135" s="34"/>
-      <c r="P135" s="34"/>
-      <c r="Q135" s="34"/>
-      <c r="R135" s="35"/>
+      <c r="B135" s="30"/>
+      <c r="C135" s="30"/>
+      <c r="D135" s="30"/>
+      <c r="E135" s="30"/>
+      <c r="F135" s="30"/>
+      <c r="G135" s="30"/>
+      <c r="H135" s="30"/>
+      <c r="I135" s="30"/>
+      <c r="J135" s="30"/>
+      <c r="K135" s="30"/>
+      <c r="L135" s="30"/>
+      <c r="M135" s="30"/>
+      <c r="N135" s="30"/>
+      <c r="O135" s="30"/>
+      <c r="P135" s="30"/>
+      <c r="Q135" s="30"/>
+      <c r="R135" s="31"/>
     </row>
     <row r="136" spans="1:18" ht="20" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="36" t="s">
+      <c r="A136" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B136" s="37"/>
-      <c r="C136" s="37"/>
-      <c r="D136" s="37"/>
-      <c r="E136" s="37"/>
-      <c r="F136" s="37"/>
-      <c r="G136" s="37"/>
-      <c r="H136" s="37"/>
-      <c r="I136" s="37"/>
-      <c r="J136" s="37"/>
-      <c r="K136" s="37"/>
-      <c r="L136" s="37"/>
-      <c r="M136" s="37"/>
-      <c r="N136" s="37"/>
-      <c r="O136" s="37"/>
-      <c r="P136" s="37"/>
-      <c r="Q136" s="37"/>
-      <c r="R136" s="38"/>
+      <c r="B136" s="33"/>
+      <c r="C136" s="33"/>
+      <c r="D136" s="33"/>
+      <c r="E136" s="33"/>
+      <c r="F136" s="33"/>
+      <c r="G136" s="33"/>
+      <c r="H136" s="33"/>
+      <c r="I136" s="33"/>
+      <c r="J136" s="33"/>
+      <c r="K136" s="33"/>
+      <c r="L136" s="33"/>
+      <c r="M136" s="33"/>
+      <c r="N136" s="33"/>
+      <c r="O136" s="33"/>
+      <c r="P136" s="33"/>
+      <c r="Q136" s="33"/>
+      <c r="R136" s="34"/>
     </row>
     <row r="137" spans="1:18" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A137" s="11">
@@ -6424,49 +6333,49 @@
     <mergeCell ref="A100:R100"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:C14 C17:C26 C29:C38 C41:C50 C53:C62 C65:C74 C77:C86 C89:C98 C101:C110 C113:C122 C125:C134 C137:C146">
-    <cfRule type="containsText" dxfId="33" priority="10" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="12" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F14 F17:F26 F29:F38 F41:F50 F53:F62 F65:F74 F77:F86 F89:F98 F101:F110 F113:F122 F125:F134 F137:F146">
-    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="8" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="9" operator="containsText" text="Not Started">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Not Started">
       <formula>NOT(ISERROR(SEARCH("Not Started",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K26 K29:K38 K41:K50 K53:K62 K65:K74 K77:K86 K89:K98 K101:K110 K113:K122 K125:K134 K137:K146 K5:K14">
-    <cfRule type="expression" dxfId="27" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>IF($K5="", 0, IF(AND($K5&lt;TODAY(), OR($L5="", $L5="N"), OR($F5="", $F5="Not Started", $F5="In Progress", $F5="On Hold")), 1, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:M26 M29:M38 M41:M50 M53:M62 M65:M74 M77:M86 M89:M98 M101:M110 M113:M122 M125:M134 M137:M146 M5:M14">
-    <cfRule type="expression" dxfId="26" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>IF($M5="", 0, IF(AND($M5&lt;TODAY(), OR($N5="", $N5="N"), OR($F5="", $F5="Not Started", $F5="In Progress", $F5="On Hold")), 1, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O17:O26 O29:O38 O41:O50 O53:O62 O65:O74 O77:O86 O89:O98 O101:O110 O113:O122 O125:O134 O137:O146 O5:O14">
-    <cfRule type="expression" dxfId="25" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>IF($O5="", 0, IF(AND($O5&lt;TODAY(), OR($P5="", $P5="N"), OR($F5="", $F5="Not Started", $F5="In Progress", $F5="On Hold")), 1, 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14 D17:D26 D29:D38 D41:D50 D53:D62 D65:D74 D77:D86 D89:D98 D101:D110 D113:D122 D125:D134 D137:D146">
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>IF(AND(NOT(ISBLANK($D5)), $D5&lt;TODAY(), $F5="Not Started"), 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E14 E17:E26 E29:E38 E41:E50 E53:E62 E65:E74 E77:E86 E89:E98 E101:E110 E113:E122 E125:E134 E137:E146">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>IF($E5="", 0, IF(AND(OR($F5="Not Started", $F5="", $F5="In Progress", $F5="On Hold"), $E5&lt;TODAY()), 1, 0))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>